<commit_message>
fix #815 : Dropped possibility to read and export Axis and Group objects from/to CSV and Excel files
</commit_message>
<xml_diff>
--- a/larray/tests/data/demography_eurostat.xlsx
+++ b/larray/tests/data/demography_eurostat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ald\Projects\larray\larray\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8679C482-EB29-4999-8BCB-CA13C13019B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1A56F9-56F3-4B57-B7D8-5D629DDE1AAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="12735" activeTab="7" xr2:uid="{239DC48C-B532-4305-8AA1-156D96EFFC20}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="12735" activeTab="5" xr2:uid="{239DC48C-B532-4305-8AA1-156D96EFFC20}"/>
   </bookViews>
   <sheets>
     <sheet name="__metadata__" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,6 @@
     <sheet name="births" sheetId="4" r:id="rId4"/>
     <sheet name="deaths" sheetId="5" r:id="rId5"/>
     <sheet name="immigration" sheetId="6" r:id="rId6"/>
-    <sheet name="__axes__" sheetId="7" r:id="rId7"/>
-    <sheet name="__groups__" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="15">
   <si>
     <t>metadata</t>
   </si>
@@ -83,18 +81,6 @@
   </si>
   <si>
     <t>citizenship</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>even_years@time</t>
-  </si>
-  <si>
-    <t>odd_years@time</t>
   </si>
 </sst>
 </file>
@@ -1178,7 +1164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F321D3A5-7537-4E22-98F2-7D18BC1AC578}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1679,134 +1665,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71E26DD2-D3BD-4D0F-AD80-5DEC9A31EC46}">
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E5">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E6">
-        <v>2017</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4064E08-187C-47E9-B6E4-77B3E20183AC}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2014</v>
-      </c>
-      <c r="B2">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2016</v>
-      </c>
-      <c r="B3">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>2017</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added new array population_5_countries in the demography_eurostat dataset
</commit_message>
<xml_diff>
--- a/larray/tests/data/demography_eurostat.xlsx
+++ b/larray/tests/data/demography_eurostat.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ald\Projects\larray\larray\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C82AE513-CFD5-42F8-9AEB-A8767187BB1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADFEDDD8-6498-426F-A299-31B6EF09BA1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="12675" activeTab="5" xr2:uid="{A20F361E-8A76-48D0-B07B-0B86558C56D3}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="12675" activeTab="6" xr2:uid="{32CD7EF8-9BC0-4813-A910-712AA1B7A6EB}"/>
   </bookViews>
   <sheets>
     <sheet name="__metadata__" sheetId="1" r:id="rId1"/>
     <sheet name="population" sheetId="2" r:id="rId2"/>
     <sheet name="population_benelux" sheetId="3" r:id="rId3"/>
-    <sheet name="births" sheetId="4" r:id="rId4"/>
-    <sheet name="deaths" sheetId="5" r:id="rId5"/>
-    <sheet name="immigration" sheetId="6" r:id="rId6"/>
+    <sheet name="population_5_countries" sheetId="4" r:id="rId4"/>
+    <sheet name="births" sheetId="5" r:id="rId5"/>
+    <sheet name="deaths" sheetId="6" r:id="rId6"/>
+    <sheet name="immigration" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="15">
   <si>
     <t>metadata</t>
   </si>
@@ -431,7 +432,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DBE9FCB-F098-4A5F-AFD4-A87FBFE531C6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B8F8494-32AE-4F4A-91CD-E45701EE6FFD}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -465,7 +466,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EBE15CA-0399-4D2F-946D-D67074225C97}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C3A1B00-D09B-463B-B89D-44C11E7AABA9}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -639,7 +640,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA6F8CD-5A8F-4062-A50D-C70FE180041F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{606FB5BF-3286-4B9A-BE47-F7BFA3DC9CE7}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -813,7 +814,273 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52B58ECE-B65C-4A75-A0BC-68FB842B1FA5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38DFD4D7-0387-4E05-8769-0CA6F0067BEB}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1">
+        <v>2013</v>
+      </c>
+      <c r="D1">
+        <v>2014</v>
+      </c>
+      <c r="E1">
+        <v>2015</v>
+      </c>
+      <c r="F1">
+        <v>2016</v>
+      </c>
+      <c r="G1">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>5472856</v>
+      </c>
+      <c r="D2">
+        <v>5493792</v>
+      </c>
+      <c r="E2">
+        <v>5524068</v>
+      </c>
+      <c r="F2">
+        <v>5569264</v>
+      </c>
+      <c r="G2">
+        <v>5589272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>5665118</v>
+      </c>
+      <c r="D3">
+        <v>5687048</v>
+      </c>
+      <c r="E3">
+        <v>5713206</v>
+      </c>
+      <c r="F3">
+        <v>5741853</v>
+      </c>
+      <c r="G3">
+        <v>5762455</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>31772665</v>
+      </c>
+      <c r="D4">
+        <v>32045129</v>
+      </c>
+      <c r="E4">
+        <v>32174258</v>
+      </c>
+      <c r="F4">
+        <v>32247386</v>
+      </c>
+      <c r="G4">
+        <v>32318973</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>33827685</v>
+      </c>
+      <c r="D5">
+        <v>34120851</v>
+      </c>
+      <c r="E5">
+        <v>34283895</v>
+      </c>
+      <c r="F5">
+        <v>34391005</v>
+      </c>
+      <c r="G5">
+        <v>34485148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>39380976</v>
+      </c>
+      <c r="D6">
+        <v>39556923</v>
+      </c>
+      <c r="E6">
+        <v>39835457</v>
+      </c>
+      <c r="F6">
+        <v>40514123</v>
+      </c>
+      <c r="G6">
+        <v>40697118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>41142770</v>
+      </c>
+      <c r="D7">
+        <v>41210540</v>
+      </c>
+      <c r="E7">
+        <v>41362080</v>
+      </c>
+      <c r="F7">
+        <v>41661561</v>
+      </c>
+      <c r="G7">
+        <v>41824535</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>268412</v>
+      </c>
+      <c r="D8">
+        <v>275117</v>
+      </c>
+      <c r="E8">
+        <v>281972</v>
+      </c>
+      <c r="F8">
+        <v>289193</v>
+      </c>
+      <c r="G8">
+        <v>296641</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>268627</v>
+      </c>
+      <c r="D9">
+        <v>274563</v>
+      </c>
+      <c r="E9">
+        <v>280986</v>
+      </c>
+      <c r="F9">
+        <v>287056</v>
+      </c>
+      <c r="G9">
+        <v>294026</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>8307339</v>
+      </c>
+      <c r="D10">
+        <v>8334385</v>
+      </c>
+      <c r="E10">
+        <v>8372858</v>
+      </c>
+      <c r="F10">
+        <v>8417135</v>
+      </c>
+      <c r="G10">
+        <v>8475102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>8472236</v>
+      </c>
+      <c r="D11">
+        <v>8494904</v>
+      </c>
+      <c r="E11">
+        <v>8527868</v>
+      </c>
+      <c r="F11">
+        <v>8561985</v>
+      </c>
+      <c r="G11">
+        <v>8606405</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB07D83-60FC-4D21-8A7F-7F3796F08F69}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -986,8 +1253,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DB538A-2610-4379-8B83-AAC9FBDFC83D}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6AFBFEA-7BCD-462C-9BC1-C52084DA8F41}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1160,8 +1427,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845CFC51-BD49-457D-BAE4-E42E139FA600}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56519ECF-2077-4961-806C-5CDEC67304F3}">
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>